<commit_message>
A table has been added with information on how information systems are literally named in the contract.
</commit_message>
<xml_diff>
--- a/Parameters/CrossingIS.xlsx
+++ b/Parameters/CrossingIS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dim-Dim\MyData\Common Work Place\Projects\DES.LM.Reports\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879FA681-C746-4034-A89B-DCF2CC4D1033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037D6B2A-C28F-46BC-AB9D-6F6B914A8034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-2730" windowWidth="29040" windowHeight="15840" xr2:uid="{C3BF7246-E3FB-429E-99E1-135FEA7739D7}"/>
   </bookViews>
@@ -38,13 +38,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>ShortPName</t>
-  </si>
-  <si>
     <t>DESLM_Project</t>
   </si>
   <si>
     <t>ISDogName</t>
+  </si>
+  <si>
+    <t>ID_DES.LM_project</t>
   </si>
 </sst>
 </file>
@@ -425,24 +425,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1E46417-8A35-48B2-8A48-58C428082082}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
     <col min="2" max="2" width="26.28515625" customWidth="1"/>
     <col min="3" max="3" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>